<commit_message>
Update scaling mapping files and metadata typo
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_scaling_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13480" yWindow="200" windowWidth="16940" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -346,8 +346,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -510,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -588,6 +594,9 @@
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -665,6 +674,9 @@
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1001,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:A63"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1041,7 +1053,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1051,7 +1063,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update EMEP mapping w/ heat included with power. Add mapping file with SO2-specific scaling rules.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_scaling_mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
@@ -346,8 +346,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -516,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -597,6 +599,7 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -677,6 +680,7 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1013,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1063,7 +1067,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Updates to scaling mappings, including limiting scaling where data has issues.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_scaling_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25640" windowHeight="19500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -89,18 +89,9 @@
     <t>1A3b_Road</t>
   </si>
   <si>
-    <t>1A3ai_International-aviation</t>
-  </si>
-  <si>
-    <t>1A3aii_Domestic-aviation</t>
-  </si>
-  <si>
     <t>1A3c_Rail</t>
   </si>
   <si>
-    <t>1A3di_International-shipping</t>
-  </si>
-  <si>
     <t>1A3dii_Domestic-naviation</t>
   </si>
   <si>
@@ -152,9 +143,6 @@
     <t>3D_Soil-emissions</t>
   </si>
   <si>
-    <t>3F_Agricultural-residue-burning-on-fields</t>
-  </si>
-  <si>
     <t>5A_Solid-waste-disposal</t>
   </si>
   <si>
@@ -173,54 +161,15 @@
     <t>A_PublicPower</t>
   </si>
   <si>
-    <t>B_Industry</t>
-  </si>
-  <si>
-    <t>C_OtherStatComb</t>
-  </si>
-  <si>
-    <t>D_Fugitive</t>
-  </si>
-  <si>
-    <t>E_Solvents</t>
-  </si>
-  <si>
-    <t>F_RoadTransport</t>
-  </si>
-  <si>
     <t>G_Shipping</t>
   </si>
   <si>
-    <t>H_Aviation</t>
-  </si>
-  <si>
-    <t>I_Offroad</t>
-  </si>
-  <si>
-    <t>J_Waste</t>
-  </si>
-  <si>
     <t>K_AgriLivestock</t>
   </si>
   <si>
     <t>L_AgriOther</t>
   </si>
   <si>
-    <t>M_Other</t>
-  </si>
-  <si>
-    <t>N_Natural</t>
-  </si>
-  <si>
-    <t>O_AviCruise</t>
-  </si>
-  <si>
-    <t>P_IntShipping</t>
-  </si>
-  <si>
-    <t>z_Memo</t>
-  </si>
-  <si>
     <t>1A1a_Electricity-public</t>
   </si>
   <si>
@@ -254,9 +203,6 @@
     <t>Solvents</t>
   </si>
   <si>
-    <t>Road</t>
-  </si>
-  <si>
     <t>2D_Degreasing-Cleaning</t>
   </si>
   <si>
@@ -272,15 +218,9 @@
     <t>3E_Enteric-fermentation</t>
   </si>
   <si>
-    <t>Aviation</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Waste</t>
-  </si>
-  <si>
     <t>2D_Paint-application</t>
   </si>
   <si>
@@ -291,6 +231,66 @@
   </si>
   <si>
     <t>2D3_Chemical-products-manufacture-processing</t>
+  </si>
+  <si>
+    <t>B_IndustrialComb</t>
+  </si>
+  <si>
+    <t>C_SmallComb</t>
+  </si>
+  <si>
+    <t>D_IndProcess</t>
+  </si>
+  <si>
+    <t>E_Fugitive</t>
+  </si>
+  <si>
+    <t>F_Solvents</t>
+  </si>
+  <si>
+    <t>G_RoadRail</t>
+  </si>
+  <si>
+    <t>I_OffRoadMob</t>
+  </si>
+  <si>
+    <t>L_OtherWasteDisp</t>
+  </si>
+  <si>
+    <t>M_WasteWater</t>
+  </si>
+  <si>
+    <t>N_WasteIncin</t>
+  </si>
+  <si>
+    <t>R_Other</t>
+  </si>
+  <si>
+    <t>S_Natural</t>
+  </si>
+  <si>
+    <t>T_IntAviCruise</t>
+  </si>
+  <si>
+    <t>IndProcess</t>
+  </si>
+  <si>
+    <t>RoadRail</t>
+  </si>
+  <si>
+    <t>OffRoadMob</t>
+  </si>
+  <si>
+    <t>OtherWasteDisp</t>
+  </si>
+  <si>
+    <t>WasteWater</t>
+  </si>
+  <si>
+    <t>WasteIncin</t>
+  </si>
+  <si>
+    <t>1A3eii_Other-transp</t>
   </si>
 </sst>
 </file>
@@ -346,8 +346,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -518,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="237">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -600,6 +674,43 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -681,6 +792,43 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1015,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1044,20 +1192,20 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1067,7 +1215,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1077,10 +1225,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1090,309 +1238,306 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
       <c r="B24" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6">
       <c r="B25" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6">
       <c r="B28" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="B30" s="4" t="s">
-        <v>73</v>
+      <c r="B30" t="s">
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6">
       <c r="B32" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
@@ -1400,277 +1545,273 @@
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>55</v>
-      </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
-      </c>
-      <c r="D39" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>63</v>
-      </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
+      <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" t="s">
-        <v>24</v>
-      </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
+      <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D43" s="2"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6">
       <c r="B44" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D44" s="2"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6">
       <c r="B45" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D45" s="2"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="B46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" t="s">
-        <v>29</v>
-      </c>
       <c r="D46" s="2"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D47" s="2"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6">
+      <c r="B48" t="s">
+        <v>86</v>
+      </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D48" s="2"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D49" s="2"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" t="s">
+        <v>87</v>
+      </c>
       <c r="C50" t="s">
-        <v>48</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="B51" s="2"/>
-      <c r="C51" t="s">
-        <v>47</v>
-      </c>
+      <c r="E51" s="1"/>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="B52" s="2"/>
-      <c r="C52" t="s">
-        <v>45</v>
-      </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E53" s="1"/>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" t="s">
-        <v>88</v>
+      <c r="B54" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E54" s="1"/>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="4"/>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="E55" s="1"/>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="4"/>
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="2"/>
+        <v>39</v>
+      </c>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="4"/>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6">
+      <c r="A58" s="4"/>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="B59" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" t="s">
-        <v>80</v>
-      </c>
+      <c r="A59" s="4"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>61</v>
+      <c r="C60" t="s">
+        <v>44</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="2"/>
+        <v>80</v>
+      </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="C63" s="4"/>
+      <c r="C63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>81</v>
+      </c>
       <c r="C64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="C65" s="2"/>
+      <c r="A65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="4"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6">
+      <c r="C66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="4"/>
+      <c r="C67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="4"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
@@ -1696,13 +1837,11 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="4"/>
-      <c r="C73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="4"/>
-      <c r="C74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
@@ -1719,21 +1858,19 @@
       <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="2"/>
+      <c r="A77" s="4"/>
       <c r="C77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="2"/>
-      <c r="B78" s="3"/>
+      <c r="A78" s="4"/>
       <c r="C78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2"/>
-      <c r="B79" s="3"/>
       <c r="C79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -1762,14 +1899,14 @@
     <row r="83" spans="1:6">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
-      <c r="C83" s="1"/>
+      <c r="C83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
-      <c r="C84" s="1"/>
+      <c r="C84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
@@ -1783,39 +1920,45 @@
     <row r="86" spans="1:6">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
+      <c r="C86" s="1"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
+      <c r="C87" s="1"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2"/>
+      <c r="B88" s="3"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2"/>
+      <c r="B89" s="3"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6">
+      <c r="A90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6">
+      <c r="A91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6">
-      <c r="E92" s="1"/>
+      <c r="E92" s="2"/>
       <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6">
-      <c r="E93" s="1"/>
+      <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6">
@@ -1823,26 +1966,28 @@
       <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6">
-      <c r="C95" s="1"/>
+      <c r="E95" s="1"/>
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6">
+      <c r="E96" s="1"/>
       <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6">
+      <c r="C97" s="1"/>
       <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6">
       <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="2"/>
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6">
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6">
+      <c r="A101" s="2"/>
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6">
@@ -1852,13 +1997,13 @@
       <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6">
-      <c r="E104" s="1"/>
       <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6">
       <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6">
+      <c r="E106" s="1"/>
       <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6">
@@ -1883,16 +2028,22 @@
       <c r="F113" s="2"/>
     </row>
     <row r="114" spans="6:6">
-      <c r="F114" s="1"/>
+      <c r="F114" s="2"/>
     </row>
     <row r="115" spans="6:6">
-      <c r="F115" s="1"/>
+      <c r="F115" s="2"/>
     </row>
     <row r="116" spans="6:6">
       <c r="F116" s="1"/>
     </row>
-    <row r="126" spans="6:6">
-      <c r="F126" s="1"/>
+    <row r="117" spans="6:6">
+      <c r="F117" s="1"/>
+    </row>
+    <row r="118" spans="6:6">
+      <c r="F118" s="1"/>
+    </row>
+    <row r="128" spans="6:6">
+      <c r="F128" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update scaling mappings to proper format
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_scaling_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25640" windowHeight="19500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="97">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -291,6 +291,27 @@
   </si>
   <si>
     <t>1A3eii_Other-transp</t>
+  </si>
+  <si>
+    <t>select_scaling_year</t>
+  </si>
+  <si>
+    <t>start_scaling_year</t>
+  </si>
+  <si>
+    <t>end_scaling_year</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>mkd</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Don't scale to 1990-1991 drop so as to be closer to EMEP trend</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -2118,15 +2139,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2139,19 +2160,43 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>1990</v>
+      </c>
+      <c r="G2">
+        <v>2010</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>